<commit_message>
fix odds / change types stats
</commit_message>
<xml_diff>
--- a/excel/stats.xlsx
+++ b/excel/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ИМЯ\Desktop\nodes\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C47AF5A-D534-4C7E-92A4-0E3D1C109C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FAB788-73A5-415A-B3F1-5DD1D1152D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK176"/>
+  <dimension ref="A1:BK1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,185 +784,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:BK1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:BK176" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>